<commit_message>
Wrote some sections of the report and fixed the D2 input to have the correct naive Bayes calculations
</commit_message>
<xml_diff>
--- a/Data/D2_LWA_Input.xlsx
+++ b/Data/D2_LWA_Input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GTech\Research\Curve Data Analytics\curve_data_analytics_python\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthew.liu\Documents\Research\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E474F2-3C78-41C5-8316-EC65A4B6898E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6EC352-A983-4721-BE81-3A20B35CF273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{524DC437-0BF5-4F4C-8031-0A4DE0B9EBF0}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{524DC437-0BF5-4F4C-8031-0A4DE0B9EBF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,8 @@
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId4"/>
-    <pivotCache cacheId="1" r:id="rId5"/>
+    <pivotCache cacheId="2" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +33,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -16058,7 +16057,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{34FF0675-2BD9-443B-AA98-432423259D65}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{34FF0675-2BD9-443B-AA98-432423259D65}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="ES1:EU18" firstHeaderRow="1" firstDataRow="1" firstDataCol="0"/>
   <pivotFields count="146">
     <pivotField showAll="0"/>
@@ -16221,458 +16220,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{41BEAB96-6698-4910-9F74-3B3AFEBA9194}" name="PivotTable7" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="AA4:AD8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="146">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="22" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField multipleItemSelectionAllowed="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisPage" showAll="0">
-      <items count="5">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="119"/>
-  </rowFields>
-  <rowItems count="3">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="9"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="30" item="3" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Count of Collision_" fld="4" subtotal="count" baseField="2" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{91E53CD8-EC4C-4C3E-BA7A-BF157D5A708D}" name="PivotTable6" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="S4:V9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
-  <pivotFields count="146">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="22" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisCol" showAll="0">
-      <items count="4">
-        <item x="1"/>
-        <item x="0"/>
-        <item x="2"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField multipleItemSelectionAllowed="1" showAll="0"/>
-    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
-      <items count="13">
-        <item h="1" x="7"/>
-        <item h="1" x="3"/>
-        <item x="4"/>
-        <item h="1" x="8"/>
-        <item h="1" x="2"/>
-        <item h="1" x="11"/>
-        <item h="1" x="5"/>
-        <item h="1" x="6"/>
-        <item x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="10"/>
-        <item h="1" x="9"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="5">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="119"/>
-  </rowFields>
-  <rowItems count="4">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="9"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </colItems>
-  <pageFields count="1">
-    <pageField fld="26" hier="-1"/>
-  </pageFields>
-  <dataFields count="1">
-    <dataField name="Count of Collision_" fld="4" subtotal="count" baseField="2" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8709ADE0-A902-4616-9902-6F3D8F188C5D}" name="PivotTable5" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8709ADE0-A902-4616-9902-6F3D8F188C5D}" name="PivotTable5" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J4:N10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="146">
     <pivotField showAll="0"/>
@@ -16898,8 +16446,8 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{66F1C9EA-B65D-4333-BBB8-A49886919643}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{66F1C9EA-B65D-4333-BBB8-A49886919643}" name="PivotTable3" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A4:E10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="146">
     <pivotField showAll="0"/>
@@ -17109,6 +16657,457 @@
       <x/>
     </i>
   </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Collision_" fld="4" subtotal="count" baseField="2" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{41BEAB96-6698-4910-9F74-3B3AFEBA9194}" name="PivotTable7" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="AA4:AD8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="146">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="22" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" showAll="0">
+      <items count="5">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="119"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="9"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="30" item="3" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of Collision_" fld="4" subtotal="count" baseField="2" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{91E53CD8-EC4C-4C3E-BA7A-BF157D5A708D}" name="PivotTable6" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="S4:V9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+  <pivotFields count="146">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="22" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="4">
+        <item x="1"/>
+        <item x="0"/>
+        <item x="2"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField multipleItemSelectionAllowed="1" showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="13">
+        <item h="1" x="7"/>
+        <item h="1" x="3"/>
+        <item x="4"/>
+        <item h="1" x="8"/>
+        <item h="1" x="2"/>
+        <item h="1" x="11"/>
+        <item h="1" x="5"/>
+        <item h="1" x="6"/>
+        <item x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="10"/>
+        <item h="1" x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="119"/>
+  </rowFields>
+  <rowItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="9"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <pageFields count="1">
+    <pageField fld="26" hier="-1"/>
+  </pageFields>
   <dataFields count="1">
     <dataField name="Count of Collision_" fld="4" subtotal="count" baseField="2" baseItem="0"/>
   </dataFields>
@@ -36285,7 +36284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31FE42F9-0EB5-4A09-B94C-48B72F995159}">
   <dimension ref="A1:EU47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -57640,8 +57639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCA58A84-B0EF-4C65-8566-FEE0B8456301}">
   <dimension ref="A1:AH10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="AG14" sqref="AG14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57661,7 +57660,9 @@
     <col min="19" max="19" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="28" max="29" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="30" max="31" width="10.77734375" bestFit="1" customWidth="1"/>
@@ -57905,16 +57906,16 @@
         <v>1</v>
       </c>
       <c r="W6">
-        <f>S6/3</f>
-        <v>0.66666666666666663</v>
+        <f>T6/3</f>
+        <v>0</v>
       </c>
       <c r="X6">
-        <f>T6/4</f>
-        <v>0</v>
+        <f>U6/4</f>
+        <v>0.25</v>
       </c>
       <c r="Y6">
         <f>IF(X6=0, 1, W6/X6)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="14">
         <v>3</v>
@@ -57927,16 +57928,16 @@
         <v>1</v>
       </c>
       <c r="AE6">
-        <f>AA6/3</f>
-        <v>1</v>
+        <f>AB6/3</f>
+        <v>0</v>
       </c>
       <c r="AF6">
-        <f>AB6/4</f>
-        <v>0</v>
+        <f>AC6/4</f>
+        <v>0.25</v>
       </c>
       <c r="AG6">
         <f>IF(AF6=0, 1, AE6/AF6)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.3">
@@ -58003,16 +58004,16 @@
         <v>3</v>
       </c>
       <c r="W7">
-        <f t="shared" ref="W7:W8" si="6">S7/3</f>
-        <v>1</v>
+        <f t="shared" ref="W7:W8" si="6">T7/3</f>
+        <v>0</v>
       </c>
       <c r="X7">
-        <f t="shared" ref="X7:X8" si="7">T7/4</f>
-        <v>0</v>
+        <f t="shared" ref="X7:X8" si="7">U7/4</f>
+        <v>0.75</v>
       </c>
       <c r="Y7">
         <f t="shared" ref="Y7:Y8" si="8">IF(X7=0, 1, W7/X7)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA7" s="14">
         <v>4</v>
@@ -58025,16 +58026,16 @@
         <v>3</v>
       </c>
       <c r="AE7">
-        <f>AA7/3</f>
-        <v>1.3333333333333333</v>
+        <f>AB7/3</f>
+        <v>1</v>
       </c>
       <c r="AF7">
-        <f t="shared" ref="AF7" si="9">AB7/4</f>
-        <v>0.75</v>
+        <f>AC7/4</f>
+        <v>0</v>
       </c>
       <c r="AG7">
-        <f t="shared" ref="AG7:AG8" si="10">IF(AF7=0, 1, AE7/AF7)</f>
-        <v>1.7777777777777777</v>
+        <f t="shared" ref="AG7:AG8" si="9">IF(AF7=0, 1, AE7/AF7)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.3">
@@ -58104,15 +58105,15 @@
       </c>
       <c r="W8">
         <f t="shared" si="6"/>
-        <v>1.6666666666666667</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="X8">
         <f t="shared" si="7"/>
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="Y8">
         <f t="shared" si="8"/>
-        <v>6.666666666666667</v>
+        <v>1</v>
       </c>
       <c r="AA8" s="14" t="s">
         <v>327</v>
@@ -58128,15 +58129,15 @@
       </c>
       <c r="AE8" s="16">
         <f>SUM(AE6:AE7)</f>
-        <v>2.333333333333333</v>
+        <v>1</v>
       </c>
       <c r="AF8" s="16">
         <f>SUM(AF6:AF7)</f>
-        <v>0.75</v>
+        <v>0.25</v>
       </c>
       <c r="AG8" s="16">
-        <f t="shared" si="10"/>
-        <v>3.1111111111111107</v>
+        <f t="shared" si="9"/>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.3">
@@ -58206,15 +58207,15 @@
       </c>
       <c r="W9" s="16">
         <f>SUM(W6:W8)</f>
-        <v>3.333333333333333</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="X9" s="16">
         <f>SUM(X6:X8)</f>
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="Y9" s="16">
         <f>IF(X9=0, 1, W9/X9)</f>
-        <v>13.333333333333332</v>
+        <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.3">
@@ -58286,9 +58287,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -58438,26 +58442,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D475958-A078-4CDC-BD7E-303003620B85}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B4114F-5715-4E58-B4E5-37E54750F1CC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39631665-2ac6-4b14-83d9-84f76f5a0db8"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -58481,9 +58474,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B4114F-5715-4E58-B4E5-37E54750F1CC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D475958-A078-4CDC-BD7E-303003620B85}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39631665-2ac6-4b14-83d9-84f76f5a0db8"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>